<commit_message>
modif journal jonas deillon
</commit_message>
<xml_diff>
--- a/documentation/3_1_Journal_Deillon_Jonas.xlsx
+++ b/documentation/3_1_Journal_Deillon_Jonas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/jonas_deillon_studentfr_ch/Documents/02.EMF/3.3eme annee/Module 306/306project/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/jonas_deillon_studentfr_ch/Documents/02.EMF/3.3eme annee/Module 306/306-G2-ArcadiaBox/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9A02705-ABC5-408A-8398-917B18788B45}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA400413-5554-4736-8B62-244355709F17}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal_DEILLON_JONAS" sheetId="8" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="20">
   <si>
     <t>Insérer les lignes au-dessus de celle-ci !</t>
   </si>
@@ -151,13 +151,25 @@
     </r>
   </si>
   <si>
-    <t>Remplisage du docuemnt BusinessCase</t>
+    <t>Cette première semaine comportait quelque peu de théorie, mais celle-ci était néanmoins nécessaire, ainsi qu’une certaine mise en place. Je trouve toujours très intéressants les projets de groupe.</t>
   </si>
   <si>
-    <t>Remplissage du docuement Cahier des charges</t>
+    <t>Daily Scrum</t>
   </si>
   <si>
-    <t>Cette première semaine comportait quelque peu de théorie, mais celle-ci était néanmoins nécessaire, ainsi qu’une certaine mise en place. Je trouve toujours très intéressants les projets de groupe.</t>
+    <t>Remplisage du document BusinessCase</t>
+  </si>
+  <si>
+    <t>Remplissage du document Cahier des charges</t>
+  </si>
+  <si>
+    <t>Documentation sur Emulator.js</t>
+  </si>
+  <si>
+    <t>Test de Emulator.js</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le sprint étant très court je n'ai pas beaucoup de réfléxion à faire mais c'était intéressant de devoir bien répartir les taches pour ce debut de projet afin doptimiser le temps mis a disposition. </t>
   </si>
 </sst>
 </file>
@@ -525,104 +537,104 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1522,21 +1534,21 @@
   <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" activePane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft"/>
       <selection activeCell="D5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="1"/>
-    <col min="2" max="3" width="31.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="217" width="9.140625" style="1" customWidth="1"/>
-    <col min="218" max="16384" width="11.5703125" style="1"/>
+    <col min="1" max="1" width="11.54296875" style="1"/>
+    <col min="2" max="3" width="31.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" style="1" customWidth="1"/>
+    <col min="5" max="217" width="9.1796875" style="1" customWidth="1"/>
+    <col min="218" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.4">
       <c r="A1" s="27" t="s">
         <v>12</v>
       </c>
@@ -1544,7 +1556,7 @@
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
     </row>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A2" s="35" t="s">
         <v>11</v>
       </c>
@@ -1554,7 +1566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>3</v>
       </c>
@@ -1566,7 +1578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="31"/>
       <c r="B5" s="31"/>
       <c r="C5" s="32"/>
@@ -1574,48 +1586,48 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="37">
+    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26">
         <v>45996</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="34"/>
       <c r="D6" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="19"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="18"/>
       <c r="D7" s="8">
         <v>1.75</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1627,46 +1639,58 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
-      <c r="B12" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-    </row>
-    <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
+    <row r="12" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+    </row>
+    <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="7">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="8">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="8">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -1675,47 +1699,49 @@
       </c>
       <c r="D18" s="9">
         <f>SUM(D13:D17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="22"/>
-    </row>
-    <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="20"/>
+      <c r="D19" s="21"/>
+    </row>
+    <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="15"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="15"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
       <c r="B25" s="2" t="s">
         <v>8</v>
       </c>
@@ -1727,44 +1753,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="15"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
-    </row>
-    <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17"/>
+    <row r="26" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="21"/>
+    </row>
+    <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="15"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="18"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="15"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19"/>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="15"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="19"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="15"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
       <c r="B32" s="2" t="s">
         <v>8</v>
       </c>
@@ -1776,44 +1802,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="23"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="26"/>
-    </row>
-    <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="14"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="17"/>
+    <row r="33" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="25"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
+    </row>
+    <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="7"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="15"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="19"/>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="18"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="15"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="18"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="15"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="19"/>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="18"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="15"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="19"/>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="18"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="15"/>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
       <c r="B39" s="2" t="s">
         <v>8</v>
       </c>
@@ -1825,44 +1851,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="23"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="26"/>
-    </row>
-    <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="14"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="17"/>
+    <row r="40" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="25"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="24"/>
+    </row>
+    <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="16"/>
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="15"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="19"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="18"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="15"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="19"/>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="14"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="18"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="15"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="19"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="14"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="18"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="15"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="19"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="14"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="18"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="15"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="14"/>
       <c r="B46" s="2" t="s">
         <v>8</v>
       </c>
@@ -1874,44 +1900,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="23"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="26"/>
-    </row>
-    <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="14"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="17"/>
+    <row r="47" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="25"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="24"/>
+    </row>
+    <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="16"/>
       <c r="D48" s="7"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="15"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="19"/>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="18"/>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="15"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="19"/>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="14"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="18"/>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="15"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="19"/>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="14"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="18"/>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="15"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="19"/>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="14"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="18"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="15"/>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
       <c r="B53" s="2" t="s">
         <v>8</v>
       </c>
@@ -1923,44 +1949,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="23"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="26"/>
-    </row>
-    <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="14"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="17"/>
+    <row r="54" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="25"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="24"/>
+    </row>
+    <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="16"/>
       <c r="D55" s="7"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="15"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="19"/>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="14"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="18"/>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="15"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="19"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="14"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="18"/>
       <c r="D57" s="8"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="15"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="19"/>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="14"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="18"/>
       <c r="D58" s="8"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="15"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="19"/>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="14"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="18"/>
       <c r="D59" s="8"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="15"/>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="14"/>
       <c r="B60" s="2" t="s">
         <v>8</v>
       </c>
@@ -1972,44 +1998,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="23"/>
-      <c r="B61" s="24"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="26"/>
-    </row>
-    <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="14"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="17"/>
+    <row r="61" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="25"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="24"/>
+    </row>
+    <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="13"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="16"/>
       <c r="D62" s="7"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="15"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="19"/>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="14"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="18"/>
       <c r="D63" s="8"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="15"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="19"/>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="14"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="18"/>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="15"/>
-      <c r="B65" s="18"/>
-      <c r="C65" s="19"/>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="14"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="18"/>
       <c r="D65" s="8"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="15"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="19"/>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="14"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="18"/>
       <c r="D66" s="8"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="15"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="14"/>
       <c r="B67" s="2" t="s">
         <v>8</v>
       </c>
@@ -2021,44 +2047,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="15"/>
-      <c r="B68" s="20"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="22"/>
-    </row>
-    <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="14"/>
-      <c r="B69" s="16"/>
-      <c r="C69" s="17"/>
+    <row r="68" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="14"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="21"/>
+    </row>
+    <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+      <c r="B69" s="15"/>
+      <c r="C69" s="16"/>
       <c r="D69" s="7"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="15"/>
-      <c r="B70" s="18"/>
-      <c r="C70" s="19"/>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="14"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="18"/>
       <c r="D70" s="8"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="15"/>
-      <c r="B71" s="18"/>
-      <c r="C71" s="19"/>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="14"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="18"/>
       <c r="D71" s="8"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="15"/>
-      <c r="B72" s="18"/>
-      <c r="C72" s="19"/>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="14"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="18"/>
       <c r="D72" s="8"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="15"/>
-      <c r="B73" s="18"/>
-      <c r="C73" s="19"/>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="14"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="18"/>
       <c r="D73" s="8"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="15"/>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="14"/>
       <c r="B74" s="2" t="s">
         <v>8</v>
       </c>
@@ -2070,44 +2096,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="23"/>
-      <c r="B75" s="24"/>
-      <c r="C75" s="25"/>
-      <c r="D75" s="26"/>
-    </row>
-    <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="14"/>
-      <c r="B76" s="16"/>
-      <c r="C76" s="17"/>
+    <row r="75" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="25"/>
+      <c r="B75" s="22"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="24"/>
+    </row>
+    <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="13"/>
+      <c r="B76" s="15"/>
+      <c r="C76" s="16"/>
       <c r="D76" s="7"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="15"/>
-      <c r="B77" s="18"/>
-      <c r="C77" s="19"/>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="14"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="18"/>
       <c r="D77" s="8"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="15"/>
-      <c r="B78" s="18"/>
-      <c r="C78" s="19"/>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="14"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="18"/>
       <c r="D78" s="8"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="15"/>
-      <c r="B79" s="18"/>
-      <c r="C79" s="19"/>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="14"/>
+      <c r="B79" s="17"/>
+      <c r="C79" s="18"/>
       <c r="D79" s="8"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="15"/>
-      <c r="B80" s="18"/>
-      <c r="C80" s="19"/>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="14"/>
+      <c r="B80" s="17"/>
+      <c r="C80" s="18"/>
       <c r="D80" s="8"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="15"/>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="14"/>
       <c r="B81" s="2" t="s">
         <v>8</v>
       </c>
@@ -2119,13 +2145,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="23"/>
-      <c r="B82" s="24"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="26"/>
-    </row>
-    <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="25"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="24"/>
+    </row>
+    <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11"/>
       <c r="B83" s="10"/>
       <c r="C83" s="3" t="s">
@@ -2133,53 +2159,51 @@
       </c>
       <c r="D83" s="12">
         <f>D11+D18+D25+D32+D39+D46+D53+D60+D67+D74+D81</f>
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="13" t="s">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="13"/>
+      <c r="B84" s="37"/>
+      <c r="C84" s="37"/>
+      <c r="D84" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="A62:A68"/>
     <mergeCell ref="B62:C62"/>
@@ -2196,38 +2220,40 @@
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B47:D47"/>
     <mergeCell ref="A48:A54"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A69:A75"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="A55:A61"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B26:D26"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D11">
     <cfRule type="containsText" dxfId="47" priority="23" operator="containsText" text="Terminé">
@@ -2351,16 +2377,16 @@
       <selection pane="bottomLeft" activeCell="B17" sqref="B17:C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="1"/>
-    <col min="2" max="3" width="31.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
-    <col min="5" max="217" width="9.140625" style="1" customWidth="1"/>
-    <col min="218" max="16384" width="11.5703125" style="1"/>
+    <col min="1" max="1" width="11.54296875" style="1"/>
+    <col min="2" max="3" width="31.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" style="1" customWidth="1"/>
+    <col min="5" max="217" width="9.1796875" style="1" customWidth="1"/>
+    <col min="218" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.4">
       <c r="A1" s="28" t="s">
         <v>1</v>
       </c>
@@ -2368,7 +2394,7 @@
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
     </row>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A2" s="35" t="s">
         <v>2</v>
       </c>
@@ -2378,7 +2404,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
         <v>3</v>
       </c>
@@ -2390,7 +2416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="31"/>
       <c r="B5" s="31"/>
       <c r="C5" s="32"/>
@@ -2398,38 +2424,38 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="37"/>
+    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26"/>
       <c r="B6" s="33"/>
       <c r="C6" s="34"/>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
@@ -2441,44 +2467,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-    </row>
-    <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
+    <row r="12" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+    </row>
+    <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -2490,44 +2516,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="22"/>
-    </row>
-    <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
+    <row r="19" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="21"/>
+    </row>
+    <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="15"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="15"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
       <c r="B25" s="2" t="s">
         <v>8</v>
       </c>
@@ -2539,44 +2565,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="15"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
-    </row>
-    <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17"/>
+    <row r="26" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="21"/>
+    </row>
+    <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="15"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="18"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="15"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19"/>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="15"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="19"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="15"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
       <c r="B32" s="2" t="s">
         <v>8</v>
       </c>
@@ -2588,44 +2614,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="23"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="26"/>
-    </row>
-    <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="14"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="17"/>
+    <row r="33" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="25"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
+    </row>
+    <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="7"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="15"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="19"/>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="14"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="18"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="15"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="18"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="15"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="19"/>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="18"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="15"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="19"/>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="18"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="15"/>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
       <c r="B39" s="2" t="s">
         <v>8</v>
       </c>
@@ -2637,44 +2663,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="23"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="26"/>
-    </row>
-    <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="14"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="17"/>
+    <row r="40" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="25"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="24"/>
+    </row>
+    <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="16"/>
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="15"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="19"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="18"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="15"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="19"/>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="14"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="18"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="15"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="19"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="14"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="18"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="15"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="19"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="14"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="18"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="15"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="14"/>
       <c r="B46" s="2" t="s">
         <v>8</v>
       </c>
@@ -2686,44 +2712,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="23"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="26"/>
-    </row>
-    <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="14"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="17"/>
+    <row r="47" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="25"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="24"/>
+    </row>
+    <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="16"/>
       <c r="D48" s="7"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="15"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="19"/>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="18"/>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="15"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="19"/>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="14"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="18"/>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="15"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="19"/>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="14"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="18"/>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="15"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="19"/>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="14"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="18"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="15"/>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
       <c r="B53" s="2" t="s">
         <v>8</v>
       </c>
@@ -2735,44 +2761,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="23"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="26"/>
-    </row>
-    <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="14"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="17"/>
+    <row r="54" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="25"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="24"/>
+    </row>
+    <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="16"/>
       <c r="D55" s="7"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="15"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="19"/>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="14"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="18"/>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="15"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="19"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="14"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="18"/>
       <c r="D57" s="8"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="15"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="19"/>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="14"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="18"/>
       <c r="D58" s="8"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="15"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="19"/>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="14"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="18"/>
       <c r="D59" s="8"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="15"/>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="14"/>
       <c r="B60" s="2" t="s">
         <v>8</v>
       </c>
@@ -2784,44 +2810,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="23"/>
-      <c r="B61" s="24"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="26"/>
-    </row>
-    <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="14"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="17"/>
+    <row r="61" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="25"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="24"/>
+    </row>
+    <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="13"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="16"/>
       <c r="D62" s="7"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="15"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="19"/>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="14"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="18"/>
       <c r="D63" s="8"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="15"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="19"/>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="14"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="18"/>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="15"/>
-      <c r="B65" s="18"/>
-      <c r="C65" s="19"/>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="14"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="18"/>
       <c r="D65" s="8"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="15"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="19"/>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="14"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="18"/>
       <c r="D66" s="8"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="15"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="14"/>
       <c r="B67" s="2" t="s">
         <v>8</v>
       </c>
@@ -2833,44 +2859,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="15"/>
-      <c r="B68" s="20"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="22"/>
-    </row>
-    <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="14"/>
-      <c r="B69" s="16"/>
-      <c r="C69" s="17"/>
+    <row r="68" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="14"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="21"/>
+    </row>
+    <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+      <c r="B69" s="15"/>
+      <c r="C69" s="16"/>
       <c r="D69" s="7"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="15"/>
-      <c r="B70" s="18"/>
-      <c r="C70" s="19"/>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="14"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="18"/>
       <c r="D70" s="8"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="15"/>
-      <c r="B71" s="18"/>
-      <c r="C71" s="19"/>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="14"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="18"/>
       <c r="D71" s="8"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="15"/>
-      <c r="B72" s="18"/>
-      <c r="C72" s="19"/>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="14"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="18"/>
       <c r="D72" s="8"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="15"/>
-      <c r="B73" s="18"/>
-      <c r="C73" s="19"/>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="14"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="18"/>
       <c r="D73" s="8"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="15"/>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="14"/>
       <c r="B74" s="2" t="s">
         <v>8</v>
       </c>
@@ -2882,44 +2908,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="23"/>
-      <c r="B75" s="24"/>
-      <c r="C75" s="25"/>
-      <c r="D75" s="26"/>
-    </row>
-    <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="14"/>
-      <c r="B76" s="16"/>
-      <c r="C76" s="17"/>
+    <row r="75" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="25"/>
+      <c r="B75" s="22"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="24"/>
+    </row>
+    <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="13"/>
+      <c r="B76" s="15"/>
+      <c r="C76" s="16"/>
       <c r="D76" s="7"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="15"/>
-      <c r="B77" s="18"/>
-      <c r="C77" s="19"/>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="14"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="18"/>
       <c r="D77" s="8"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="15"/>
-      <c r="B78" s="18"/>
-      <c r="C78" s="19"/>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="14"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="18"/>
       <c r="D78" s="8"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="15"/>
-      <c r="B79" s="18"/>
-      <c r="C79" s="19"/>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="14"/>
+      <c r="B79" s="17"/>
+      <c r="C79" s="18"/>
       <c r="D79" s="8"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="15"/>
-      <c r="B80" s="18"/>
-      <c r="C80" s="19"/>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="14"/>
+      <c r="B80" s="17"/>
+      <c r="C80" s="18"/>
       <c r="D80" s="8"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="15"/>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="14"/>
       <c r="B81" s="2" t="s">
         <v>8</v>
       </c>
@@ -2931,13 +2957,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="23"/>
-      <c r="B82" s="24"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="26"/>
-    </row>
-    <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="25"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="24"/>
+    </row>
+    <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11"/>
       <c r="B83" s="10"/>
       <c r="C83" s="3" t="s">
@@ -2948,16 +2974,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="13" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="13"/>
+      <c r="B84" s="37"/>
+      <c r="C84" s="37"/>
+      <c r="D84" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="A69:A75"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="A55:A61"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A4:A5"/>
@@ -2969,77 +3066,6 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B82:D82"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D11">
     <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="Terminé">
@@ -3163,17 +3189,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BD0882D7B13D249A8B88997E24B9140" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="3865b25f2bf2a035dbe7787239b3f11c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8afaa137-8a18-4908-97f4-35fc924e5a91" xmlns:ns3="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="718f9f7ddd2530d56a17ab9424d0abda" ns2:_="" ns3:_="">
     <xsd:import namespace="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
@@ -3386,6 +3401,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
   <ds:schemaRefs>
@@ -3395,19 +3421,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b54f96d8-6138-4ba9-8b5a-da1062324abb"/>
-    <ds:schemaRef ds:uri="0ecde9c3-6951-4ee0-98d0-295e535ef6cd"/>
-    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
-    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84AEF82B-2BAE-481D-A319-B09ADD6915E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3424,4 +3437,17 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b54f96d8-6138-4ba9-8b5a-da1062324abb"/>
+    <ds:schemaRef ds:uri="0ecde9c3-6951-4ee0-98d0-295e535ef6cd"/>
+    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
+    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
commit heures jonas 2
</commit_message>
<xml_diff>
--- a/documentation/3_1_Journal_Deillon_Jonas.xlsx
+++ b/documentation/3_1_Journal_Deillon_Jonas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\OneDrive - EDUETATFR\02.EMF\3.3eme annee\Module 306\306-G2-ArcadiaBox\306-G2-ArcadiaBox\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/jonas_deillon_studentfr_ch/Documents/02.EMF/3.3eme annee/Module 306/306-G2-ArcadiaBox/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0C8584-3F8B-4C59-B556-80744EFED626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B09B778D-3C33-4780-A0B1-3F27F52E57A0}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-180" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal_DEILLON_JONAS" sheetId="8" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="23">
   <si>
     <r>
       <rPr>
@@ -185,12 +185,6 @@
   <si>
     <t xml:space="preserve">Documentation  </t>
   </si>
-  <si>
-    <t>Mise en place su système de récupération de score</t>
-  </si>
-  <si>
-    <t>Ce sprint était assez intense, car je me suis beaucoup concentré sur une tâche jusqu’à y parvenir. Ma persévérance a mené à un résultat concluant, avec un système fonctionnel, ce qui constitue un point positif. Ce sprint était principalement axé sur la réalisation, mais nous avons également remarqué que la documentation est primordiale et que nous l’avons quelque peu négligée.</t>
-  </si>
 </sst>
 </file>
 
@@ -557,104 +551,104 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1201,6 +1195,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1554,21 +1552,21 @@
   <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft"/>
       <selection activeCell="D5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26:D26"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" style="1"/>
-    <col min="2" max="3" width="31.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7265625" style="1" customWidth="1"/>
-    <col min="5" max="217" width="9.1796875" style="1" customWidth="1"/>
-    <col min="218" max="16384" width="11.54296875" style="1"/>
+    <col min="1" max="1" width="11.5703125" style="1"/>
+    <col min="2" max="3" width="31.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5" max="217" width="9.140625" style="1" customWidth="1"/>
+    <col min="218" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
@@ -1576,7 +1574,7 @@
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
     </row>
-    <row r="2" spans="1:4" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
@@ -1586,7 +1584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>2</v>
       </c>
@@ -1598,7 +1596,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" s="31"/>
       <c r="C5" s="32"/>
@@ -1606,8 +1604,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37">
+    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="26">
         <v>45996</v>
       </c>
       <c r="B6" s="33" t="s">
@@ -1618,36 +1616,36 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="18" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="14"/>
+      <c r="B7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="19"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="8">
         <v>1.75</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="14"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="14"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="14"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="14"/>
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1659,60 +1657,60 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="20" t="s">
+    <row r="12" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="14"/>
+      <c r="B12" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-    </row>
-    <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+    </row>
+    <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="13">
         <v>46003</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="17"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="7">
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="18" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="14"/>
+      <c r="B14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="19"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="8">
         <v>0.75</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="18" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="14"/>
+      <c r="B15" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="19"/>
+      <c r="C15" s="18"/>
       <c r="D15" s="8">
         <v>0.75</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="14"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="14"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="14"/>
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -1724,64 +1722,60 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="20" t="s">
+    <row r="19" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="14"/>
+      <c r="B19" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="22"/>
-    </row>
-    <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14">
+      <c r="C19" s="20"/>
+      <c r="D19" s="21"/>
+    </row>
+    <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="13">
         <v>46009</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="17"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="7">
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="18" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="14"/>
+      <c r="B21" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="19"/>
+      <c r="C21" s="18"/>
       <c r="D21" s="8">
         <v>0.1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="18" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="14"/>
+      <c r="B22" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="19"/>
+      <c r="C22" s="18"/>
       <c r="D22" s="8">
         <v>3.2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="8">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="14"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="14"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="14"/>
       <c r="B25" s="2" t="s">
         <v>8</v>
       </c>
@@ -1790,49 +1784,47 @@
       </c>
       <c r="D25" s="9">
         <f>SUM(D20:D24)</f>
-        <v>5.3000000000000007</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
-    </row>
-    <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17"/>
+        <v>3.5500000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="14"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="21"/>
+    </row>
+    <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="13"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="14"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="18"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19"/>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="14"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="14"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="19"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="14"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="14"/>
       <c r="B32" s="2" t="s">
         <v>8</v>
       </c>
@@ -1844,44 +1836,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="26"/>
-    </row>
-    <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="17"/>
+    <row r="33" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="25"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
+    </row>
+    <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="13"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="7"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="19"/>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="14"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="18"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="14"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="18"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="19"/>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="14"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="18"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="19"/>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="14"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="18"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="14"/>
       <c r="B39" s="2" t="s">
         <v>8</v>
       </c>
@@ -1893,44 +1885,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="26"/>
-    </row>
-    <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="17"/>
+    <row r="40" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="25"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="24"/>
+    </row>
+    <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="13"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="16"/>
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="19"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="14"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="18"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="19"/>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="14"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="18"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="19"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="14"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="18"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="19"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="14"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="18"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="14"/>
       <c r="B46" s="2" t="s">
         <v>8</v>
       </c>
@@ -1942,44 +1934,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="26"/>
-    </row>
-    <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="17"/>
+    <row r="47" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="25"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="24"/>
+    </row>
+    <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="13"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="16"/>
       <c r="D48" s="7"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="19"/>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="14"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="18"/>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="19"/>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="14"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="18"/>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="19"/>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="14"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="18"/>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="19"/>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="14"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="18"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="14"/>
       <c r="B53" s="2" t="s">
         <v>8</v>
       </c>
@@ -1991,44 +1983,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="26"/>
-    </row>
-    <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="14"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="17"/>
+    <row r="54" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="25"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="24"/>
+    </row>
+    <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="13"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="16"/>
       <c r="D55" s="7"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="19"/>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="14"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="18"/>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="15"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="19"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="14"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="18"/>
       <c r="D57" s="8"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="19"/>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="14"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="18"/>
       <c r="D58" s="8"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="19"/>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="14"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="18"/>
       <c r="D59" s="8"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="15"/>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="14"/>
       <c r="B60" s="2" t="s">
         <v>8</v>
       </c>
@@ -2040,44 +2032,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
-      <c r="B61" s="24"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="26"/>
-    </row>
-    <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="17"/>
+    <row r="61" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="25"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="24"/>
+    </row>
+    <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="13"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="16"/>
       <c r="D62" s="7"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="15"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="19"/>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="14"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="18"/>
       <c r="D63" s="8"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="19"/>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="14"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="18"/>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="15"/>
-      <c r="B65" s="18"/>
-      <c r="C65" s="19"/>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="14"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="18"/>
       <c r="D65" s="8"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="19"/>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="14"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="18"/>
       <c r="D66" s="8"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="15"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="14"/>
       <c r="B67" s="2" t="s">
         <v>8</v>
       </c>
@@ -2089,44 +2081,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="15"/>
-      <c r="B68" s="20"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="22"/>
-    </row>
-    <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
-      <c r="B69" s="16"/>
-      <c r="C69" s="17"/>
+    <row r="68" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="14"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="21"/>
+    </row>
+    <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="13"/>
+      <c r="B69" s="15"/>
+      <c r="C69" s="16"/>
       <c r="D69" s="7"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
-      <c r="B70" s="18"/>
-      <c r="C70" s="19"/>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="14"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="18"/>
       <c r="D70" s="8"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="15"/>
-      <c r="B71" s="18"/>
-      <c r="C71" s="19"/>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="14"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="18"/>
       <c r="D71" s="8"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="15"/>
-      <c r="B72" s="18"/>
-      <c r="C72" s="19"/>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="14"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="18"/>
       <c r="D72" s="8"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="15"/>
-      <c r="B73" s="18"/>
-      <c r="C73" s="19"/>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="14"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="18"/>
       <c r="D73" s="8"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="15"/>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="14"/>
       <c r="B74" s="2" t="s">
         <v>8</v>
       </c>
@@ -2138,44 +2130,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="23"/>
-      <c r="B75" s="24"/>
-      <c r="C75" s="25"/>
-      <c r="D75" s="26"/>
-    </row>
-    <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
-      <c r="B76" s="16"/>
-      <c r="C76" s="17"/>
+    <row r="75" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="25"/>
+      <c r="B75" s="22"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="24"/>
+    </row>
+    <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="13"/>
+      <c r="B76" s="15"/>
+      <c r="C76" s="16"/>
       <c r="D76" s="7"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="15"/>
-      <c r="B77" s="18"/>
-      <c r="C77" s="19"/>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="14"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="18"/>
       <c r="D77" s="8"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="15"/>
-      <c r="B78" s="18"/>
-      <c r="C78" s="19"/>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="14"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="18"/>
       <c r="D78" s="8"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="15"/>
-      <c r="B79" s="18"/>
-      <c r="C79" s="19"/>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="14"/>
+      <c r="B79" s="17"/>
+      <c r="C79" s="18"/>
       <c r="D79" s="8"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="15"/>
-      <c r="B80" s="18"/>
-      <c r="C80" s="19"/>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="14"/>
+      <c r="B80" s="17"/>
+      <c r="C80" s="18"/>
       <c r="D80" s="8"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="15"/>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="14"/>
       <c r="B81" s="2" t="s">
         <v>8</v>
       </c>
@@ -2187,13 +2179,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="23"/>
-      <c r="B82" s="24"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="26"/>
-    </row>
-    <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="25"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="24"/>
+    </row>
+    <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11"/>
       <c r="B83" s="10"/>
       <c r="C83" s="3" t="s">
@@ -2201,53 +2193,51 @@
       </c>
       <c r="D83" s="12">
         <f>D11+D18+D25+D32+D39+D46+D53+D60+D67+D74+D81</f>
-        <v>10.8</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="13" t="s">
+        <v>9.0500000000000007</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="13"/>
+      <c r="B84" s="37"/>
+      <c r="C84" s="37"/>
+      <c r="D84" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="A62:A68"/>
     <mergeCell ref="B62:C62"/>
@@ -2264,38 +2254,40 @@
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B47:D47"/>
     <mergeCell ref="A48:A54"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A69:A75"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="A55:A61"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B26:D26"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D11">
     <cfRule type="containsText" dxfId="47" priority="23" operator="containsText" text="Terminé">
@@ -2419,16 +2411,16 @@
       <selection pane="bottomLeft" activeCell="B17" sqref="B17:C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" style="1"/>
-    <col min="2" max="3" width="31.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7265625" style="1" customWidth="1"/>
-    <col min="5" max="217" width="9.1796875" style="1" customWidth="1"/>
-    <col min="218" max="16384" width="11.54296875" style="1"/>
+    <col min="1" max="1" width="11.5703125" style="1"/>
+    <col min="2" max="3" width="31.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="1" customWidth="1"/>
+    <col min="5" max="217" width="9.140625" style="1" customWidth="1"/>
+    <col min="218" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
         <v>17</v>
       </c>
@@ -2436,7 +2428,7 @@
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
     </row>
-    <row r="2" spans="1:4" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>18</v>
       </c>
@@ -2446,7 +2438,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>2</v>
       </c>
@@ -2458,7 +2450,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" s="31"/>
       <c r="C5" s="32"/>
@@ -2466,38 +2458,38 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
+    <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="26"/>
       <c r="B6" s="33"/>
       <c r="C6" s="34"/>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="14"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="14"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="14"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="14"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="14"/>
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
@@ -2509,44 +2501,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-    </row>
-    <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
+    <row r="12" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="14"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+    </row>
+    <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="13"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="19"/>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="14"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="14"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="14"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="14"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="14"/>
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -2558,44 +2550,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="22"/>
-    </row>
-    <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
+    <row r="19" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="14"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="21"/>
+    </row>
+    <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="13"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="14"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="14"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="14"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="14"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="18"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="14"/>
       <c r="B25" s="2" t="s">
         <v>8</v>
       </c>
@@ -2607,44 +2599,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
-    </row>
-    <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17"/>
+    <row r="26" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="14"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="21"/>
+    </row>
+    <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="13"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19"/>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="14"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="18"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="19"/>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="14"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="18"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="19"/>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="14"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="18"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="19"/>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="14"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="18"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="14"/>
       <c r="B32" s="2" t="s">
         <v>8</v>
       </c>
@@ -2656,44 +2648,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="26"/>
-    </row>
-    <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="17"/>
+    <row r="33" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="25"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
+    </row>
+    <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="13"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="7"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="19"/>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="14"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="18"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="14"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="18"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="19"/>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="14"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="18"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="19"/>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="14"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="18"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="14"/>
       <c r="B39" s="2" t="s">
         <v>8</v>
       </c>
@@ -2705,44 +2697,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="26"/>
-    </row>
-    <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="17"/>
+    <row r="40" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="25"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="24"/>
+    </row>
+    <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="13"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="16"/>
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="19"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="14"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="18"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="19"/>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="14"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="18"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="19"/>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="14"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="18"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="19"/>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="14"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="18"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="14"/>
       <c r="B46" s="2" t="s">
         <v>8</v>
       </c>
@@ -2754,44 +2746,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="26"/>
-    </row>
-    <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="17"/>
+    <row r="47" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="25"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="24"/>
+    </row>
+    <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="13"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="16"/>
       <c r="D48" s="7"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="19"/>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="14"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="18"/>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="19"/>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="14"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="18"/>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
-      <c r="B51" s="18"/>
-      <c r="C51" s="19"/>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="14"/>
+      <c r="B51" s="17"/>
+      <c r="C51" s="18"/>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="19"/>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="14"/>
+      <c r="B52" s="17"/>
+      <c r="C52" s="18"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="14"/>
       <c r="B53" s="2" t="s">
         <v>8</v>
       </c>
@@ -2803,44 +2795,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="26"/>
-    </row>
-    <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="14"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="17"/>
+    <row r="54" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="25"/>
+      <c r="B54" s="22"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="24"/>
+    </row>
+    <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="13"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="16"/>
       <c r="D55" s="7"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="19"/>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="14"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="18"/>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="15"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="19"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="14"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="18"/>
       <c r="D57" s="8"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="19"/>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="14"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="18"/>
       <c r="D58" s="8"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="19"/>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="14"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="18"/>
       <c r="D59" s="8"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="15"/>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="14"/>
       <c r="B60" s="2" t="s">
         <v>8</v>
       </c>
@@ -2852,44 +2844,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
-      <c r="B61" s="24"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="26"/>
-    </row>
-    <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="17"/>
+    <row r="61" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="25"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="24"/>
+    </row>
+    <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="13"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="16"/>
       <c r="D62" s="7"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="15"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="19"/>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="14"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="18"/>
       <c r="D63" s="8"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="19"/>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="14"/>
+      <c r="B64" s="17"/>
+      <c r="C64" s="18"/>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="15"/>
-      <c r="B65" s="18"/>
-      <c r="C65" s="19"/>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="14"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="18"/>
       <c r="D65" s="8"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="19"/>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="14"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="18"/>
       <c r="D66" s="8"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="15"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="14"/>
       <c r="B67" s="2" t="s">
         <v>8</v>
       </c>
@@ -2901,44 +2893,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="15"/>
-      <c r="B68" s="20"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="22"/>
-    </row>
-    <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
-      <c r="B69" s="16"/>
-      <c r="C69" s="17"/>
+    <row r="68" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="14"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="21"/>
+    </row>
+    <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="13"/>
+      <c r="B69" s="15"/>
+      <c r="C69" s="16"/>
       <c r="D69" s="7"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
-      <c r="B70" s="18"/>
-      <c r="C70" s="19"/>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="14"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="18"/>
       <c r="D70" s="8"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="15"/>
-      <c r="B71" s="18"/>
-      <c r="C71" s="19"/>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="14"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="18"/>
       <c r="D71" s="8"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="15"/>
-      <c r="B72" s="18"/>
-      <c r="C72" s="19"/>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="14"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="18"/>
       <c r="D72" s="8"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="15"/>
-      <c r="B73" s="18"/>
-      <c r="C73" s="19"/>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="14"/>
+      <c r="B73" s="17"/>
+      <c r="C73" s="18"/>
       <c r="D73" s="8"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="15"/>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="14"/>
       <c r="B74" s="2" t="s">
         <v>8</v>
       </c>
@@ -2950,44 +2942,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="23"/>
-      <c r="B75" s="24"/>
-      <c r="C75" s="25"/>
-      <c r="D75" s="26"/>
-    </row>
-    <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
-      <c r="B76" s="16"/>
-      <c r="C76" s="17"/>
+    <row r="75" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="25"/>
+      <c r="B75" s="22"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="24"/>
+    </row>
+    <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="13"/>
+      <c r="B76" s="15"/>
+      <c r="C76" s="16"/>
       <c r="D76" s="7"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="15"/>
-      <c r="B77" s="18"/>
-      <c r="C77" s="19"/>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="14"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="18"/>
       <c r="D77" s="8"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="15"/>
-      <c r="B78" s="18"/>
-      <c r="C78" s="19"/>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="14"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="18"/>
       <c r="D78" s="8"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="15"/>
-      <c r="B79" s="18"/>
-      <c r="C79" s="19"/>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="14"/>
+      <c r="B79" s="17"/>
+      <c r="C79" s="18"/>
       <c r="D79" s="8"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="15"/>
-      <c r="B80" s="18"/>
-      <c r="C80" s="19"/>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="14"/>
+      <c r="B80" s="17"/>
+      <c r="C80" s="18"/>
       <c r="D80" s="8"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="15"/>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="14"/>
       <c r="B81" s="2" t="s">
         <v>8</v>
       </c>
@@ -2999,13 +2991,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="23"/>
-      <c r="B82" s="24"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="26"/>
-    </row>
-    <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="25"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="24"/>
+    </row>
+    <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11"/>
       <c r="B83" s="10"/>
       <c r="C83" s="3" t="s">
@@ -3016,16 +3008,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="13" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="13"/>
+      <c r="B84" s="37"/>
+      <c r="C84" s="37"/>
+      <c r="D84" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="A69:A75"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="A55:A61"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="A13:A19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A4:A5"/>
@@ -3037,77 +3100,6 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B12:D12"/>
-    <mergeCell ref="A13:A19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B82:D82"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D11">
     <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="Terminé">
@@ -3222,26 +3214,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BD0882D7B13D249A8B88997E24B9140" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="3865b25f2bf2a035dbe7787239b3f11c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8afaa137-8a18-4908-97f4-35fc924e5a91" xmlns:ns3="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="718f9f7ddd2530d56a17ab9424d0abda" ns2:_="" ns3:_="">
     <xsd:import namespace="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
@@ -3454,10 +3426,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84AEF82B-2BAE-481D-A319-B09ADD6915E9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
+    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3474,20 +3477,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84AEF82B-2BAE-481D-A319-B09ADD6915E9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
-    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
commit heure jonas definitif
</commit_message>
<xml_diff>
--- a/documentation/3_1_Journal_Deillon_Jonas.xlsx
+++ b/documentation/3_1_Journal_Deillon_Jonas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduetatfr-my.sharepoint.com/personal/jonas_deillon_studentfr_ch/Documents/02.EMF/3.3eme annee/Module 306/306-G2-ArcadiaBox/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\stu.net.fr.ch\perso$\Users\deillonj04\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{C68E2980-A969-4E78-98D4-6A7237E3E30A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B09B778D-3C33-4780-A0B1-3F27F52E57A0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D04856-16F0-41BE-B657-A52BE9C83EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-180" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="26">
   <si>
     <r>
       <rPr>
@@ -185,6 +185,15 @@
   <si>
     <t xml:space="preserve">Documentation  </t>
   </si>
+  <si>
+    <t>Mise en place su système de récupération de score</t>
+  </si>
+  <si>
+    <t>Ce sprint était assez intense, car je me suis beaucoup concentré sur une tâche jusqu’à y parvenir. Ma persévérance a mené à un résultat concluant, avec un système fonctionnel, ce qui constitue un point positif. Ce sprint était principalement axé sur la réalisation, mais nous avons également remarqué que la documentation est primordiale et que nous l’avons quelque peu négligée.</t>
+  </si>
+  <si>
+    <t>Implémentation du l'émulateur en production</t>
+  </si>
 </sst>
 </file>
 
@@ -655,29 +664,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="46">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1195,10 +1182,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1551,10 +1534,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft"/>
       <selection activeCell="D5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1764,9 +1747,6 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="14"/>
@@ -1789,21 +1769,33 @@
     </row>
     <row r="26" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="14"/>
-      <c r="B26" s="19"/>
+      <c r="B26" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="C26" s="20"/>
       <c r="D26" s="21"/>
     </row>
     <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="7"/>
+      <c r="A27" s="13">
+        <v>46010</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="8">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="14"/>
-      <c r="B28" s="17"/>
+      <c r="B28" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="C28" s="18"/>
-      <c r="D28" s="8"/>
+      <c r="D28" s="8">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="14"/>
@@ -1833,7 +1825,7 @@
       </c>
       <c r="D32" s="9">
         <f>SUM(D27:D31)</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -2193,7 +2185,7 @@
       </c>
       <c r="D83" s="12">
         <f>D11+D18+D25+D32+D39+D46+D53+D60+D67+D74+D81</f>
-        <v>9.0500000000000007</v>
+        <v>15.55</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -2205,7 +2197,7 @@
       <c r="D84" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="82">
+  <mergeCells count="81">
     <mergeCell ref="A84:D84"/>
     <mergeCell ref="A13:A19"/>
     <mergeCell ref="B13:C13"/>
@@ -2215,7 +2207,6 @@
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
@@ -2285,32 +2276,24 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B27:C27"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B26:D26"/>
   </mergeCells>
-  <conditionalFormatting sqref="D6:D11">
-    <cfRule type="containsText" dxfId="47" priority="23" operator="containsText" text="Terminé">
+  <conditionalFormatting sqref="D6:D11 D20:D22 D24:D25 D27">
+    <cfRule type="containsText" dxfId="45" priority="23" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="24" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="44" priority="24" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:D18">
-    <cfRule type="containsText" dxfId="45" priority="21" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="43" priority="21" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="22" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="42" priority="22" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D20:D25">
-    <cfRule type="containsText" dxfId="43" priority="3" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="4" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:D32">
@@ -3214,6 +3197,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BD0882D7B13D249A8B88997E24B9140" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="3865b25f2bf2a035dbe7787239b3f11c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8afaa137-8a18-4908-97f4-35fc924e5a91" xmlns:ns3="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="718f9f7ddd2530d56a17ab9424d0abda" ns2:_="" ns3:_="">
     <xsd:import namespace="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
@@ -3426,7 +3418,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
@@ -3437,16 +3429,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84AEF82B-2BAE-481D-A319-B09ADD6915E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3465,7 +3456,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3474,12 +3465,4 @@
     <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>